<commit_message>
Update job title form via API
</commit_message>
<xml_diff>
--- a/job_titles.xlsx
+++ b/job_titles.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Job_Title</t>
   </si>
   <si>
     <t>Fullstack Developer</t>
+  </si>
+  <si>
+    <t>Dotnet Developer</t>
   </si>
 </sst>
 </file>
@@ -377,7 +380,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -393,6 +396,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>